<commit_message>
add validate param middleware
</commit_message>
<xml_diff>
--- a/back-end-loto-app/output/excelBuild.xlsx
+++ b/back-end-loto-app/output/excelBuild.xlsx
@@ -397,61 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <v>4</v>
-      </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
-      <c r="F1">
-        <v>6</v>
-      </c>
-      <c r="G1">
-        <v>7</v>
-      </c>
-      <c r="H1">
-        <v>8</v>
-      </c>
-      <c r="I1">
-        <v>9</v>
-      </c>
-      <c r="J1">
-        <v>10</v>
-      </c>
-      <c r="K1">
-        <v>11</v>
-      </c>
-      <c r="L1">
-        <v>12</v>
-      </c>
-      <c r="M1">
-        <v>13</v>
-      </c>
-      <c r="N1">
-        <v>14</v>
-      </c>
-      <c r="O1">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>